<commit_message>
Fix: Ensure data persistence using Named Volumes
</commit_message>
<xml_diff>
--- a/Liste.xlsx
+++ b/Liste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\CodeGradeAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{37E1E97B-805B-450B-BF82-6330D1D7FC33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{229C4E6C-30EC-4BEE-A24F-E304CAF7A712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4992" yWindow="4992" windowWidth="34560" windowHeight="18600" xr2:uid="{0818A35B-D0EF-4139-A8E6-35B3EF8C07F0}"/>
+    <workbookView xWindow="29028" yWindow="3888" windowWidth="13032" windowHeight="18600" xr2:uid="{0818A35B-D0EF-4139-A8E6-35B3EF8C07F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>OgrenciNo</t>
   </si>
@@ -96,6 +96,12 @@
   </si>
   <si>
     <t>Ayşa</t>
+  </si>
+  <si>
+    <t>Canlı</t>
+  </si>
+  <si>
+    <t>Berk</t>
   </si>
 </sst>
 </file>
@@ -154,10 +160,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -494,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52F2044F-0B01-40F7-B87D-1C177077AE87}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -611,10 +617,24 @@
         <v>19</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>20251006</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>